<commit_message>
Save all data to excel
</commit_message>
<xml_diff>
--- a/lib/standards.xlsx
+++ b/lib/standards.xlsx
@@ -81,15 +81,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="33.0" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="25.3" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="28.6" min="2" max="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -110,7 +114,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Daryl Holcomb</t>
+          <t>Adam Rodgers</t>
         </is>
       </c>
     </row>
@@ -122,7 +126,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Deserunt in rem ut i</t>
+          <t>Omnis minus ut iste </t>
         </is>
       </c>
     </row>
@@ -133,7 +137,7 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2002</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="6">
@@ -144,7 +148,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Aperiam commodi comm</t>
+          <t>Laborum Consectetur</t>
         </is>
       </c>
     </row>
@@ -154,10 +158,8 @@
           <t>Created at</t>
         </is>
       </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B7" s="2">
+        <v>45690.64534295795</v>
       </c>
     </row>
     <row r="8">
@@ -166,10 +168,8 @@
           <t>Updated at</t>
         </is>
       </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B8" s="2">
+        <v>45692.01832649687</v>
       </c>
     </row>
     <row r="9">
@@ -203,15 +203,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="48.400000000000006" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="25.3" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="28.6" min="2" max="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -232,7 +236,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>UL</t>
         </is>
       </c>
     </row>
@@ -243,7 +247,7 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>22</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -253,7 +257,7 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>401</v>
+        <v>601</v>
       </c>
     </row>
     <row r="6">
@@ -263,7 +267,7 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>472</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7">
@@ -273,7 +277,7 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>100</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -283,7 +287,7 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -293,7 +297,7 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -303,7 +307,7 @@
         </is>
       </c>
       <c r="B10" s="0" t="n">
-        <v>78</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -314,7 +318,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Cupiditate quaerat q</t>
+          <t>Esse blanditiis mol</t>
         </is>
       </c>
     </row>
@@ -325,7 +329,7 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13">
@@ -335,7 +339,7 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -345,7 +349,7 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
@@ -355,7 +359,7 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
@@ -366,7 +370,7 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Voluptate a rerum se</t>
+          <t>Voluptatum dolore si</t>
         </is>
       </c>
     </row>
@@ -378,7 +382,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>Sint et deserunt et </t>
+          <t>Velit vel dolor non</t>
         </is>
       </c>
     </row>
@@ -390,7 +394,7 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>Ducimus vel distinc</t>
+          <t>Aut voluptas nihil e</t>
         </is>
       </c>
     </row>
@@ -401,7 +405,7 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
@@ -411,7 +415,7 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21">
@@ -420,10 +424,8 @@
           <t>Created at</t>
         </is>
       </c>
-      <c r="B21" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B21" s="2">
+        <v>45690.64534335464</v>
       </c>
     </row>
     <row r="22">
@@ -432,10 +434,8 @@
           <t>Updated at</t>
         </is>
       </c>
-      <c r="B22" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B22" s="2">
+        <v>45692.01832656486</v>
       </c>
     </row>
     <row r="23">
@@ -469,15 +469,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="33.0" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="25.3" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="28.6" min="2" max="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -498,7 +502,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Odit facere omnis si</t>
+          <t>Unde labore assumend</t>
         </is>
       </c>
     </row>
@@ -510,7 +514,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Qui dolor accusantiu</t>
+          <t>Mollitia excepturi v</t>
         </is>
       </c>
     </row>
@@ -522,7 +526,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Rerum et ea quae ver</t>
+          <t>Rerum sit dolor qua</t>
         </is>
       </c>
     </row>
@@ -533,7 +537,7 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1973</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="7">
@@ -544,7 +548,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Ut velit reprehender</t>
+          <t>Temporibus do obcaec</t>
         </is>
       </c>
     </row>
@@ -556,7 +560,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Do aute laboris aspe</t>
+          <t>Iusto quae irure cil</t>
         </is>
       </c>
     </row>
@@ -568,7 +572,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Reprehenderit aliqu</t>
+          <t>Eum autem aliquam la</t>
         </is>
       </c>
     </row>
@@ -588,10 +592,8 @@
           <t>Created at</t>
         </is>
       </c>
-      <c r="B11" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B11" s="2">
+        <v>45690.645347796984</v>
       </c>
     </row>
     <row r="12">
@@ -600,10 +602,8 @@
           <t>Updated at</t>
         </is>
       </c>
-      <c r="B12" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B12" s="2">
+        <v>45692.0183270467</v>
       </c>
     </row>
   </sheetData>
@@ -627,15 +627,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="33.0" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="25.3" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="28.6" min="2" max="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -656,7 +660,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Laborum Eius sit s</t>
+          <t>Nisi quis esse vero</t>
         </is>
       </c>
     </row>
@@ -668,7 +672,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>In libero rerum labo</t>
+          <t>Quae dolor proident</t>
         </is>
       </c>
     </row>
@@ -680,7 +684,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Est dicta voluptas f</t>
+          <t>Culpa et totam elig</t>
         </is>
       </c>
     </row>
@@ -692,7 +696,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Tenetur non consecte</t>
+          <t>Labore odit enim qui</t>
         </is>
       </c>
     </row>
@@ -704,7 +708,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Ipsa dolores adipis</t>
+          <t>Excepturi voluptas q</t>
         </is>
       </c>
     </row>
@@ -724,10 +728,8 @@
           <t>Created at</t>
         </is>
       </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B9" s="2">
+        <v>45690.64534860172</v>
       </c>
     </row>
     <row r="10">
@@ -736,10 +738,8 @@
           <t>Updated at</t>
         </is>
       </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B10" s="2">
+        <v>45692.01832712396</v>
       </c>
     </row>
   </sheetData>
@@ -763,27 +763,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="59.400000000000006" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="5.5" min="2" max="2" bestFit="1" customWidth="1"/>
-    <col width="5.5" min="3" max="3" bestFit="1" customWidth="1"/>
-    <col width="7.700000000000001" min="4" max="4" bestFit="1" customWidth="1"/>
+    <col width="8.8" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="13.200000000000001" min="3" max="3" bestFit="1" customWidth="1"/>
+    <col width="9.9" min="4" max="4" bestFit="1" customWidth="1"/>
     <col width="25.3" min="5" max="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>5</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Unit Rate</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -793,17 +803,17 @@
         </is>
       </c>
       <c r="B2" s="0" t="n">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>4316</v>
+        <v>5166</v>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Quam voluptatem labo</t>
+          <t>Quis ut est minima </t>
         </is>
       </c>
     </row>
@@ -814,17 +824,17 @@
         </is>
       </c>
       <c r="B3" s="0" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>4018</v>
+        <v>3666</v>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Exercitationem dolor</t>
+          <t>Lorem sunt sit dolor</t>
         </is>
       </c>
     </row>
@@ -835,17 +845,17 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1440</v>
+        <v>6888</v>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>Possimus reprehende</t>
+          <t>Deserunt suscipit es</t>
         </is>
       </c>
     </row>
@@ -856,17 +866,17 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>4794</v>
+        <v>2535</v>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>Exercitationem quos </t>
+          <t>Facilis aut dolores </t>
         </is>
       </c>
     </row>
@@ -877,17 +887,17 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1350</v>
+        <v>4704</v>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>Natus dignissimos ni</t>
+          <t>Veritatis consectetu</t>
         </is>
       </c>
     </row>
@@ -898,17 +908,17 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>360</v>
+        <v>1863</v>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>Ut dolor ad voluptat</t>
+          <t>Laboriosam tempore</t>
         </is>
       </c>
     </row>
@@ -919,17 +929,17 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>806</v>
+        <v>1924</v>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>Rem occaecat nostrum</t>
+          <t>Dolor est aut autem</t>
         </is>
       </c>
     </row>
@@ -940,17 +950,17 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>6664</v>
+        <v>528</v>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>Minim veritatis est </t>
+          <t>Repudiandae nobis cu</t>
         </is>
       </c>
     </row>
@@ -961,17 +971,17 @@
         </is>
       </c>
       <c r="B10" s="0" t="n">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>3864</v>
+        <v>44</v>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>Sint quis magni in </t>
+          <t>Deleniti sed et sit </t>
         </is>
       </c>
     </row>
@@ -982,17 +992,17 @@
         </is>
       </c>
       <c r="B11" s="0" t="n">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>3312</v>
+        <v>1649</v>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>Corporis corrupti a</t>
+          <t>Ea enim ipsam fugiat</t>
         </is>
       </c>
     </row>
@@ -1003,17 +1013,17 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>34</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>68</v>
+        <v>1462</v>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>Porro non sint est </t>
+          <t>Amet quis dolores i</t>
         </is>
       </c>
     </row>
@@ -1024,17 +1034,17 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>160</v>
+        <v>4760</v>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>Consequatur volupta</t>
+          <t>Qui nemo delectus e</t>
         </is>
       </c>
     </row>
@@ -1045,17 +1055,17 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1936</v>
+        <v>6438</v>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>Eligendi aliquip vol</t>
+          <t>Et voluptate nemo Na</t>
         </is>
       </c>
     </row>
@@ -1066,17 +1076,17 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>390</v>
+        <v>805</v>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>Quia inventore sed s</t>
+          <t>Sunt quisquam mollit</t>
         </is>
       </c>
     </row>
@@ -1087,17 +1097,17 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>5152</v>
+        <v>8900</v>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>Quo perspiciatis si</t>
+          <t>Occaecat voluptatem</t>
         </is>
       </c>
     </row>
@@ -1108,17 +1118,17 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>2714</v>
+        <v>1334</v>
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>Dolor consequatur ne</t>
+          <t>Reprehenderit cupid</t>
         </is>
       </c>
     </row>
@@ -1129,17 +1139,17 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>756</v>
+        <v>2244</v>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>Officia commodi null</t>
+          <t>Velit sequi odio mo</t>
         </is>
       </c>
     </row>
@@ -1150,17 +1160,17 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>3021</v>
+        <v>4088</v>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>Omnis saepe ut in se</t>
+          <t>Temporibus qui repel</t>
         </is>
       </c>
     </row>
@@ -1171,17 +1181,17 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>4059</v>
+        <v>273</v>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>Velit aliquip in eiu</t>
+          <t>Sequi nulla ad volup</t>
         </is>
       </c>
     </row>
@@ -1192,17 +1202,17 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>720</v>
+        <v>2747</v>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>Sed culpa voluptate</t>
+          <t>Deserunt et dolorem </t>
         </is>
       </c>
     </row>
@@ -1227,15 +1237,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="30.800000000000004" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="25.3" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="28.6" min="2" max="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1256,7 +1270,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Repudiandae voluptas</t>
+          <t>Ut aperiam esse dict</t>
         </is>
       </c>
     </row>
@@ -1296,10 +1310,8 @@
           <t>Created at</t>
         </is>
       </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B7" s="2">
+        <v>45690.645346053454</v>
       </c>
     </row>
     <row r="8">
@@ -1308,10 +1320,8 @@
           <t>Updated at</t>
         </is>
       </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B8" s="2">
+        <v>45692.01832689102</v>
       </c>
     </row>
   </sheetData>
@@ -1335,27 +1345,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="28.6" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="4.4" min="2" max="2" bestFit="1" customWidth="1"/>
-    <col width="4.4" min="3" max="3" bestFit="1" customWidth="1"/>
-    <col width="4.4" min="4" max="4" bestFit="1" customWidth="1"/>
-    <col width="4.4" min="5" max="5" bestFit="1" customWidth="1"/>
+    <col width="8.8" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="13.200000000000001" min="3" max="3" bestFit="1" customWidth="1"/>
+    <col width="9.9" min="4" max="4" bestFit="1" customWidth="1"/>
+    <col width="24.200000000000003" min="5" max="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>5</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Unit Rate</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1364,24 +1384,18 @@
           <t>Total Number of Devices</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="B2" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>6240</v>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>Sint saepe aliqua </t>
         </is>
       </c>
     </row>
@@ -1391,24 +1405,18 @@
           <t>Total Number of Relays</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>168</v>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>Dolor sit non ratio</t>
         </is>
       </c>
     </row>
@@ -1433,15 +1441,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col width="36.300000000000004" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="25.3" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="28.6" min="2" max="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Key</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1462,7 +1474,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Ut temporibus repreh</t>
+          <t>Amet illo ea eum au</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1485,7 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
@@ -1493,7 +1505,7 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -1503,7 +1515,7 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>83</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -1513,7 +1525,7 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -1523,7 +1535,7 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>200</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
@@ -1542,10 +1554,8 @@
           <t>Created at</t>
         </is>
       </c>
-      <c r="B11" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B11" s="2">
+        <v>45690.645349403334</v>
       </c>
     </row>
     <row r="12">
@@ -1554,10 +1564,8 @@
           <t>Updated at</t>
         </is>
       </c>
-      <c r="B12" s="0" t="inlineStr">
-        <is>
-          <t>2025-02-02</t>
-        </is>
+      <c r="B12" s="2">
+        <v>45692.018326822916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>